<commit_message>
changed vendor name and updated screenshots
</commit_message>
<xml_diff>
--- a/invoice/invoice_worksheet_v1.xlsx
+++ b/invoice/invoice_worksheet_v1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hao\Desktop\comoto_invoice_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hao\Desktop\Hao Dong io\haodong191.github.io\invoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD01E40-25A4-4647-8196-A3901FA0C883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4FCFC6-41F7-42F6-818B-6BFD2CAB4318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="147">
   <si>
     <t>Input</t>
   </si>
@@ -498,6 +498,9 @@
   </si>
   <si>
     <t>Total Extra Value</t>
+  </si>
+  <si>
+    <t>Rider’s Depot</t>
   </si>
 </sst>
 </file>
@@ -847,7 +850,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -875,36 +878,34 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -922,30 +923,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -966,29 +943,25 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1009,22 +982,43 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1312,7 +1306,7 @@
   <dimension ref="A1:AB81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z36" sqref="Z36"/>
+      <selection activeCell="N2" activeCellId="1" sqref="G1:G1048576 N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,7 +1324,7 @@
     <col min="11" max="11" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.140625" style="2" bestFit="1" customWidth="1"/>
@@ -1343,44 +1337,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="57" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="15" t="s">
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="20" t="s">
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="21" t="s">
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1422,7 +1416,7 @@
       <c r="M2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="13" t="s">
         <v>5</v>
       </c>
       <c r="O2" s="3" t="s">
@@ -1437,23 +1431,23 @@
       <c r="R2" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="S2" s="19" t="s">
+      <c r="S2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19" t="s">
+      <c r="T2" s="3"/>
+      <c r="U2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="V2" s="19" t="s">
+      <c r="V2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="19"/>
-      <c r="X2" s="30" t="s">
+      <c r="W2" s="3"/>
+      <c r="X2" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="30"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
@@ -1476,7 +1470,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H3" s="3">
         <v>10427570</v>
@@ -1497,8 +1491,8 @@
       <c r="M3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="17" t="s">
-        <v>6</v>
+      <c r="N3" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O3">
         <f>IFERROR(INDEX(A:A, MATCH(H3, A:A, 0)), "No Match")</f>
@@ -1532,10 +1526,10 @@
         <v>2799.9600000000005</v>
       </c>
       <c r="W3" s="2"/>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="30"/>
-      <c r="Z3" s="30"/>
-      <c r="AA3" s="30"/>
+      <c r="X3" s="49"/>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="49"/>
+      <c r="AA3" s="49"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -1558,7 +1552,7 @@
         <v>17</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H4" s="3">
         <v>10427190</v>
@@ -1579,8 +1573,8 @@
       <c r="M4" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="N4" s="17" t="s">
-        <v>6</v>
+      <c r="N4" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O4">
         <f t="shared" ref="O4:O57" si="2">IFERROR(INDEX(A:A, MATCH(H4, A:A, 0)), "No Match")</f>
@@ -1613,14 +1607,13 @@
         <v>1679.9760000000001</v>
       </c>
       <c r="W4" s="2"/>
-      <c r="X4" s="34">
+      <c r="X4" s="51">
         <f>SUM(J1:J100) / SUM(C1:C100)</f>
         <v>0.5734526472781506</v>
       </c>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="35"/>
-      <c r="AA4" s="36"/>
-      <c r="AB4" s="31"/>
+      <c r="Y4" s="52"/>
+      <c r="Z4" s="52"/>
+      <c r="AA4" s="53"/>
     </row>
     <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
@@ -1643,7 +1636,7 @@
         <v>18</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H5" s="3">
         <v>10377115</v>
@@ -1664,8 +1657,8 @@
       <c r="M5" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="N5" s="17" t="s">
-        <v>6</v>
+      <c r="N5" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O5">
         <f t="shared" si="2"/>
@@ -1697,11 +1690,11 @@
         <f t="shared" si="4"/>
         <v>4479.9360000000006</v>
       </c>
-      <c r="W5" s="33"/>
-      <c r="X5" s="37"/>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
-      <c r="AA5" s="39"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="55"/>
+      <c r="Z5" s="55"/>
+      <c r="AA5" s="56"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -1724,7 +1717,7 @@
         <v>19</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H6" s="3">
         <v>10427184</v>
@@ -1745,8 +1738,8 @@
       <c r="M6" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="N6" s="17" t="s">
-        <v>6</v>
+      <c r="N6" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O6">
         <f t="shared" si="2"/>
@@ -1779,12 +1772,12 @@
         <v>559.99200000000008</v>
       </c>
       <c r="W6" s="2"/>
-      <c r="X6" s="30" t="s">
+      <c r="X6" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="Y6" s="30"/>
-      <c r="Z6" s="30"/>
-      <c r="AA6" s="30"/>
+      <c r="Y6" s="49"/>
+      <c r="Z6" s="49"/>
+      <c r="AA6" s="49"/>
     </row>
     <row r="7" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
@@ -1807,7 +1800,7 @@
         <v>20</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H7" s="3">
         <v>10427567</v>
@@ -1828,8 +1821,8 @@
       <c r="M7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N7" s="17" t="s">
-        <v>6</v>
+      <c r="N7" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O7">
         <f t="shared" si="2"/>
@@ -1862,10 +1855,10 @@
         <v>1119.9840000000002</v>
       </c>
       <c r="W7" s="2"/>
-      <c r="X7" s="30"/>
-      <c r="Y7" s="30"/>
-      <c r="Z7" s="30"/>
-      <c r="AA7" s="30"/>
+      <c r="X7" s="49"/>
+      <c r="Y7" s="49"/>
+      <c r="Z7" s="49"/>
+      <c r="AA7" s="49"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -1888,7 +1881,7 @@
         <v>21</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H8" s="3">
         <v>10377105</v>
@@ -1909,8 +1902,8 @@
       <c r="M8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N8" s="17" t="s">
-        <v>6</v>
+      <c r="N8" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O8">
         <f t="shared" si="2"/>
@@ -1938,14 +1931,13 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X8" s="40">
+      <c r="X8" s="30">
         <f>SUM(L1:L100)</f>
         <v>356870.82850000024</v>
       </c>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="42"/>
-      <c r="AB8" s="31"/>
+      <c r="Y8" s="31"/>
+      <c r="Z8" s="31"/>
+      <c r="AA8" s="32"/>
     </row>
     <row r="9" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
@@ -1968,7 +1960,7 @@
         <v>22</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H9" s="3">
         <v>10427161</v>
@@ -1989,8 +1981,8 @@
       <c r="M9" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="N9" s="17" t="s">
-        <v>6</v>
+      <c r="N9" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O9">
         <f t="shared" si="2"/>
@@ -2018,11 +2010,10 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X9" s="43"/>
-      <c r="Y9" s="44"/>
-      <c r="Z9" s="44"/>
-      <c r="AA9" s="45"/>
-      <c r="AB9" s="31"/>
+      <c r="X9" s="33"/>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="34"/>
+      <c r="AA9" s="35"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -2045,7 +2036,7 @@
         <v>23</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H10" s="11">
         <v>10377106</v>
@@ -2066,8 +2057,8 @@
       <c r="M10" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="N10" s="17" t="s">
-        <v>6</v>
+      <c r="N10" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O10">
         <f t="shared" si="2"/>
@@ -2095,10 +2086,10 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X10" s="32"/>
-      <c r="Y10" s="32"/>
-      <c r="Z10" s="32"/>
-      <c r="AA10" s="32"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="16"/>
+      <c r="AA10" s="16"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -2121,7 +2112,7 @@
         <v>24</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H11" s="3">
         <v>10377116</v>
@@ -2142,8 +2133,8 @@
       <c r="M11" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="N11" s="17" t="s">
-        <v>6</v>
+      <c r="N11" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O11">
         <f t="shared" si="2"/>
@@ -2171,12 +2162,12 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X11" s="54" t="s">
+      <c r="X11" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="Y11" s="54"/>
-      <c r="Z11" s="54"/>
-      <c r="AA11" s="54"/>
+      <c r="Y11" s="36"/>
+      <c r="Z11" s="36"/>
+      <c r="AA11" s="36"/>
     </row>
     <row r="12" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
@@ -2199,7 +2190,7 @@
         <v>25</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H12" s="3">
         <v>10427185</v>
@@ -2220,8 +2211,8 @@
       <c r="M12" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="N12" s="17" t="s">
-        <v>6</v>
+      <c r="N12" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O12">
         <f t="shared" si="2"/>
@@ -2249,10 +2240,10 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X12" s="54"/>
-      <c r="Y12" s="54"/>
-      <c r="Z12" s="54"/>
-      <c r="AA12" s="54"/>
+      <c r="X12" s="36"/>
+      <c r="Y12" s="36"/>
+      <c r="Z12" s="36"/>
+      <c r="AA12" s="36"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -2275,7 +2266,7 @@
         <v>26</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H13" s="3">
         <v>10427568</v>
@@ -2296,8 +2287,8 @@
       <c r="M13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="17" t="s">
-        <v>6</v>
+      <c r="N13" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O13">
         <f t="shared" si="2"/>
@@ -2325,13 +2316,13 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X13" s="61">
+      <c r="X13" s="37">
         <f>SUM(C1:C100) / SUM(J1:J100) - 1</f>
         <v>0.74382314694408325</v>
       </c>
-      <c r="Y13" s="62"/>
-      <c r="Z13" s="62"/>
-      <c r="AA13" s="63"/>
+      <c r="Y13" s="38"/>
+      <c r="Z13" s="38"/>
+      <c r="AA13" s="39"/>
     </row>
     <row r="14" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
@@ -2354,7 +2345,7 @@
         <v>27</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H14" s="3">
         <v>10427187</v>
@@ -2375,8 +2366,8 @@
       <c r="M14" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="N14" s="17" t="s">
-        <v>6</v>
+      <c r="N14" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
@@ -2404,10 +2395,10 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X14" s="64"/>
-      <c r="Y14" s="65"/>
-      <c r="Z14" s="65"/>
-      <c r="AA14" s="66"/>
+      <c r="X14" s="40"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="41"/>
+      <c r="AA14" s="42"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -2430,7 +2421,7 @@
         <v>28</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H15" s="3">
         <v>10457332</v>
@@ -2451,8 +2442,8 @@
       <c r="M15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="17" t="s">
-        <v>6</v>
+      <c r="N15" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O15">
         <f t="shared" si="2"/>
@@ -2480,12 +2471,12 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X15" s="54" t="s">
+      <c r="X15" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="Y15" s="54"/>
-      <c r="Z15" s="54"/>
-      <c r="AA15" s="54"/>
+      <c r="Y15" s="36"/>
+      <c r="Z15" s="36"/>
+      <c r="AA15" s="36"/>
     </row>
     <row r="16" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
@@ -2508,7 +2499,7 @@
         <v>29</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H16" s="3">
         <v>10377114</v>
@@ -2529,8 +2520,8 @@
       <c r="M16" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="N16" s="17" t="s">
-        <v>6</v>
+      <c r="N16" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O16">
         <f t="shared" si="2"/>
@@ -2558,10 +2549,10 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X16" s="54"/>
-      <c r="Y16" s="54"/>
-      <c r="Z16" s="54"/>
-      <c r="AA16" s="54"/>
+      <c r="X16" s="36"/>
+      <c r="Y16" s="36"/>
+      <c r="Z16" s="36"/>
+      <c r="AA16" s="36"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -2584,7 +2575,7 @@
         <v>30</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H17" s="3">
         <v>10427167</v>
@@ -2605,8 +2596,8 @@
       <c r="M17" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="N17" s="17" t="s">
-        <v>6</v>
+      <c r="N17" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O17">
         <f t="shared" si="2"/>
@@ -2634,13 +2625,13 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X17" s="55">
+      <c r="X17" s="43">
         <f>SUM(E1:E100) - SUM(L1:L100)</f>
         <v>183610.2329999996</v>
       </c>
-      <c r="Y17" s="56"/>
-      <c r="Z17" s="56"/>
-      <c r="AA17" s="57"/>
+      <c r="Y17" s="44"/>
+      <c r="Z17" s="44"/>
+      <c r="AA17" s="45"/>
     </row>
     <row r="18" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
@@ -2663,7 +2654,7 @@
         <v>31</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H18" s="3">
         <v>10427164</v>
@@ -2684,8 +2675,8 @@
       <c r="M18" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="N18" s="17" t="s">
-        <v>6</v>
+      <c r="N18" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O18">
         <f t="shared" si="2"/>
@@ -2713,10 +2704,10 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X18" s="58"/>
-      <c r="Y18" s="59"/>
-      <c r="Z18" s="59"/>
-      <c r="AA18" s="60"/>
+      <c r="X18" s="46"/>
+      <c r="Y18" s="47"/>
+      <c r="Z18" s="47"/>
+      <c r="AA18" s="48"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -2739,7 +2730,7 @@
         <v>32</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H19" s="3">
         <v>10427565</v>
@@ -2760,8 +2751,8 @@
       <c r="M19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N19" s="17" t="s">
-        <v>6</v>
+      <c r="N19" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O19">
         <f t="shared" si="2"/>
@@ -2789,10 +2780,10 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X19" s="46"/>
-      <c r="Y19" s="46"/>
-      <c r="Z19" s="46"/>
-      <c r="AA19" s="46"/>
+      <c r="X19" s="16"/>
+      <c r="Y19" s="16"/>
+      <c r="Z19" s="16"/>
+      <c r="AA19" s="16"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -2815,7 +2806,7 @@
         <v>33</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H20" s="3">
         <v>10427160</v>
@@ -2836,8 +2827,8 @@
       <c r="M20" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="N20" s="17" t="s">
-        <v>6</v>
+      <c r="N20" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O20">
         <f t="shared" si="2"/>
@@ -2865,12 +2856,12 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X20" s="47" t="s">
+      <c r="X20" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="Y20" s="47"/>
-      <c r="Z20" s="47"/>
-      <c r="AA20" s="47"/>
+      <c r="Y20" s="17"/>
+      <c r="Z20" s="17"/>
+      <c r="AA20" s="17"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
@@ -2893,7 +2884,7 @@
         <v>34</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H21" s="3">
         <v>10427191</v>
@@ -2914,8 +2905,8 @@
       <c r="M21" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="N21" s="17" t="s">
-        <v>6</v>
+      <c r="N21" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O21">
         <f t="shared" si="2"/>
@@ -2943,10 +2934,10 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X21" s="47"/>
-      <c r="Y21" s="47"/>
-      <c r="Z21" s="47"/>
-      <c r="AA21" s="47"/>
+      <c r="X21" s="17"/>
+      <c r="Y21" s="17"/>
+      <c r="Z21" s="17"/>
+      <c r="AA21" s="17"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -2969,7 +2960,7 @@
         <v>35</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H22" s="3">
         <v>10427566</v>
@@ -2977,10 +2968,10 @@
       <c r="I22" s="3">
         <v>8980210905</v>
       </c>
-      <c r="J22" s="23">
+      <c r="J22" s="3">
         <v>7</v>
       </c>
-      <c r="K22" s="22">
+      <c r="K22" s="15">
         <v>149.49350000000001</v>
       </c>
       <c r="L22" s="8">
@@ -2990,8 +2981,8 @@
       <c r="M22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N22" s="17" t="s">
-        <v>6</v>
+      <c r="N22" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O22">
         <f t="shared" si="2"/>
@@ -3019,13 +3010,13 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X22" s="48" cm="1">
+      <c r="X22" s="18" cm="1">
         <f t="array" ref="X22">SUM(IF(ISNUMBER(U:U), U:U, 0))</f>
         <v>19</v>
       </c>
-      <c r="Y22" s="49"/>
-      <c r="Z22" s="49"/>
-      <c r="AA22" s="50"/>
+      <c r="Y22" s="19"/>
+      <c r="Z22" s="19"/>
+      <c r="AA22" s="20"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
@@ -3048,7 +3039,7 @@
         <v>36</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H23" s="3">
         <v>10427576</v>
@@ -3069,8 +3060,8 @@
       <c r="M23" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N23" s="17" t="s">
-        <v>6</v>
+      <c r="N23" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O23">
         <f t="shared" si="2"/>
@@ -3098,10 +3089,10 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X23" s="51"/>
-      <c r="Y23" s="52"/>
-      <c r="Z23" s="52"/>
-      <c r="AA23" s="53"/>
+      <c r="X23" s="21"/>
+      <c r="Y23" s="22"/>
+      <c r="Z23" s="22"/>
+      <c r="AA23" s="23"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -3124,7 +3115,7 @@
         <v>37</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H24" s="3">
         <v>10377094</v>
@@ -3145,8 +3136,8 @@
       <c r="M24" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="N24" s="17" t="s">
-        <v>6</v>
+      <c r="N24" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O24">
         <f t="shared" si="2"/>
@@ -3174,12 +3165,12 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X24" s="47" t="s">
+      <c r="X24" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="Y24" s="47"/>
-      <c r="Z24" s="47"/>
-      <c r="AA24" s="47"/>
+      <c r="Y24" s="17"/>
+      <c r="Z24" s="17"/>
+      <c r="AA24" s="17"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
@@ -3202,7 +3193,7 @@
         <v>38</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H25" s="3">
         <v>10457328</v>
@@ -3223,8 +3214,8 @@
       <c r="M25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N25" s="17" t="s">
-        <v>6</v>
+      <c r="N25" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O25">
         <f t="shared" si="2"/>
@@ -3252,10 +3243,10 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="X25" s="47"/>
-      <c r="Y25" s="47"/>
-      <c r="Z25" s="47"/>
-      <c r="AA25" s="47"/>
+      <c r="X25" s="17"/>
+      <c r="Y25" s="17"/>
+      <c r="Z25" s="17"/>
+      <c r="AA25" s="17"/>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
@@ -3278,7 +3269,7 @@
         <v>63</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H26" s="3">
         <v>10377107</v>
@@ -3299,8 +3290,8 @@
       <c r="M26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="N26" s="17" t="s">
-        <v>6</v>
+      <c r="N26" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O26">
         <f t="shared" si="2"/>
@@ -3357,7 +3348,7 @@
         <v>64</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H27" s="3">
         <v>10427170</v>
@@ -3378,8 +3369,8 @@
       <c r="M27" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="N27" s="17" t="s">
-        <v>6</v>
+      <c r="N27" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O27">
         <f t="shared" si="2"/>
@@ -3433,7 +3424,7 @@
         <v>65</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H28" s="3">
         <v>10377096</v>
@@ -3454,8 +3445,8 @@
       <c r="M28" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N28" s="17" t="s">
-        <v>6</v>
+      <c r="N28" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O28">
         <f t="shared" si="2"/>
@@ -3505,7 +3496,7 @@
         <v>66</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H29" s="3">
         <v>10427563</v>
@@ -3526,8 +3517,8 @@
       <c r="M29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N29" s="17" t="s">
-        <v>6</v>
+      <c r="N29" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O29">
         <f t="shared" si="2"/>
@@ -3577,7 +3568,7 @@
         <v>67</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H30" s="3">
         <v>10377112</v>
@@ -3598,8 +3589,8 @@
       <c r="M30" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="N30" s="17" t="s">
-        <v>6</v>
+      <c r="N30" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O30">
         <f t="shared" si="2"/>
@@ -3649,7 +3640,7 @@
         <v>68</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H31" s="3">
         <v>10377111</v>
@@ -3670,8 +3661,8 @@
       <c r="M31" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N31" s="17" t="s">
-        <v>6</v>
+      <c r="N31" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O31">
         <f t="shared" si="2"/>
@@ -3721,7 +3712,7 @@
         <v>69</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H32" s="3">
         <v>10427571</v>
@@ -3742,8 +3733,8 @@
       <c r="M32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N32" s="17" t="s">
-        <v>6</v>
+      <c r="N32" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O32">
         <f t="shared" si="2"/>
@@ -3793,7 +3784,7 @@
         <v>70</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H33" s="3">
         <v>10427188</v>
@@ -3814,8 +3805,8 @@
       <c r="M33" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="N33" s="17" t="s">
-        <v>6</v>
+      <c r="N33" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O33">
         <f t="shared" si="2"/>
@@ -3865,7 +3856,7 @@
         <v>71</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H34" s="3">
         <v>10377104</v>
@@ -3886,8 +3877,8 @@
       <c r="M34" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="N34" s="17" t="s">
-        <v>6</v>
+      <c r="N34" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O34">
         <f t="shared" si="2"/>
@@ -3937,7 +3928,7 @@
         <v>72</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H35" s="3">
         <v>10377109</v>
@@ -3958,8 +3949,8 @@
       <c r="M35" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="N35" s="17" t="s">
-        <v>6</v>
+      <c r="N35" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O35">
         <f t="shared" si="2"/>
@@ -4009,7 +4000,7 @@
         <v>73</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H36" s="3">
         <v>10377103</v>
@@ -4030,8 +4021,8 @@
       <c r="M36" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="N36" s="17" t="s">
-        <v>6</v>
+      <c r="N36" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O36">
         <f t="shared" si="2"/>
@@ -4081,7 +4072,7 @@
         <v>74</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H37" s="3">
         <v>10427165</v>
@@ -4102,8 +4093,8 @@
       <c r="M37" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="N37" s="17" t="s">
-        <v>6</v>
+      <c r="N37" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O37">
         <f t="shared" si="2"/>
@@ -4153,7 +4144,7 @@
         <v>75</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H38" s="3">
         <v>10457330</v>
@@ -4174,8 +4165,8 @@
       <c r="M38" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N38" s="17" t="s">
-        <v>6</v>
+      <c r="N38" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O38">
         <f t="shared" si="2"/>
@@ -4225,7 +4216,7 @@
         <v>76</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H39" s="3">
         <v>10427163</v>
@@ -4246,8 +4237,8 @@
       <c r="M39" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="N39" s="17" t="s">
-        <v>6</v>
+      <c r="N39" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O39">
         <f t="shared" si="2"/>
@@ -4297,7 +4288,7 @@
         <v>77</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H40" s="3">
         <v>10427569</v>
@@ -4318,8 +4309,8 @@
       <c r="M40" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N40" s="17" t="s">
-        <v>6</v>
+      <c r="N40" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O40">
         <f t="shared" si="2"/>
@@ -4369,7 +4360,7 @@
         <v>78</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H41" s="3">
         <v>10377101</v>
@@ -4390,8 +4381,8 @@
       <c r="M41" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="N41" s="17" t="s">
-        <v>6</v>
+      <c r="N41" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O41">
         <f t="shared" si="2"/>
@@ -4441,7 +4432,7 @@
         <v>79</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H42" s="3">
         <v>10457333</v>
@@ -4462,8 +4453,8 @@
       <c r="M42" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N42" s="17" t="s">
-        <v>6</v>
+      <c r="N42" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O42">
         <f t="shared" si="2"/>
@@ -4513,7 +4504,7 @@
         <v>80</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H43" s="3">
         <v>10377098</v>
@@ -4534,8 +4525,8 @@
       <c r="M43" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="N43" s="17" t="s">
-        <v>6</v>
+      <c r="N43" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O43">
         <f t="shared" si="2"/>
@@ -4585,7 +4576,7 @@
         <v>81</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H44" s="3">
         <v>10377102</v>
@@ -4606,8 +4597,8 @@
       <c r="M44" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="N44" s="17" t="s">
-        <v>6</v>
+      <c r="N44" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O44">
         <f t="shared" si="2"/>
@@ -4657,7 +4648,7 @@
         <v>82</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H45" s="3">
         <v>10427189</v>
@@ -4678,8 +4669,8 @@
       <c r="M45" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="N45" s="17" t="s">
-        <v>6</v>
+      <c r="N45" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O45">
         <f t="shared" si="2"/>
@@ -4729,7 +4720,7 @@
         <v>83</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H46" s="3">
         <v>10377097</v>
@@ -4750,8 +4741,8 @@
       <c r="M46" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N46" s="17" t="s">
-        <v>6</v>
+      <c r="N46" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O46">
         <f t="shared" si="2"/>
@@ -4801,7 +4792,7 @@
         <v>84</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H47" s="3">
         <v>10377100</v>
@@ -4822,8 +4813,8 @@
       <c r="M47" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="N47" s="17" t="s">
-        <v>6</v>
+      <c r="N47" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O47">
         <f t="shared" si="2"/>
@@ -4873,7 +4864,7 @@
         <v>85</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H48" s="3">
         <v>10427171</v>
@@ -4894,8 +4885,8 @@
       <c r="M48" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="N48" s="17" t="s">
-        <v>6</v>
+      <c r="N48" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O48">
         <f t="shared" si="2"/>
@@ -4945,7 +4936,7 @@
         <v>86</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H49" s="3">
         <v>10427162</v>
@@ -4966,8 +4957,8 @@
       <c r="M49" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="N49" s="17" t="s">
-        <v>6</v>
+      <c r="N49" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O49">
         <f t="shared" si="2"/>
@@ -5017,7 +5008,7 @@
         <v>87</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H50" s="3">
         <v>10427173</v>
@@ -5038,8 +5029,8 @@
       <c r="M50" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N50" s="17" t="s">
-        <v>6</v>
+      <c r="N50" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O50">
         <f t="shared" si="2"/>
@@ -5089,7 +5080,7 @@
         <v>88</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H51" s="3">
         <v>10377093</v>
@@ -5110,8 +5101,8 @@
       <c r="M51" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N51" s="17" t="s">
-        <v>6</v>
+      <c r="N51" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O51">
         <f t="shared" si="2"/>
@@ -5151,7 +5142,7 @@
         <v>89</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H52" s="3">
         <v>10427575</v>
@@ -5172,8 +5163,8 @@
       <c r="M52" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N52" s="17" t="s">
-        <v>6</v>
+      <c r="N52" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O52">
         <f t="shared" si="2"/>
@@ -5213,7 +5204,7 @@
         <v>90</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H53">
         <v>10353748</v>
@@ -5234,8 +5225,8 @@
       <c r="M53" t="s">
         <v>133</v>
       </c>
-      <c r="N53" s="17" t="s">
-        <v>6</v>
+      <c r="N53" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O53" t="str">
         <f>IFERROR(INDEX(A:A, MATCH(H53, A:A, 0)), "No Match")</f>
@@ -5275,7 +5266,7 @@
         <v>91</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H54">
         <v>10353749</v>
@@ -5296,8 +5287,8 @@
       <c r="M54" t="s">
         <v>134</v>
       </c>
-      <c r="N54" s="17" t="s">
-        <v>6</v>
+      <c r="N54" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O54" t="str">
         <f t="shared" si="2"/>
@@ -5337,7 +5328,7 @@
         <v>92</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H55">
         <v>10353750</v>
@@ -5358,8 +5349,8 @@
       <c r="M55" t="s">
         <v>135</v>
       </c>
-      <c r="N55" s="17" t="s">
-        <v>6</v>
+      <c r="N55" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O55" t="str">
         <f t="shared" si="2"/>
@@ -5399,7 +5390,7 @@
         <v>93</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H56">
         <v>10353751</v>
@@ -5420,8 +5411,8 @@
       <c r="M56" t="s">
         <v>136</v>
       </c>
-      <c r="N56" s="17" t="s">
-        <v>6</v>
+      <c r="N56" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O56" t="str">
         <f t="shared" si="2"/>
@@ -5461,7 +5452,7 @@
         <v>94</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="H57">
         <v>10353752</v>
@@ -5482,8 +5473,8 @@
       <c r="M57" t="s">
         <v>137</v>
       </c>
-      <c r="N57" s="17" t="s">
-        <v>6</v>
+      <c r="N57" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="O57" t="str">
         <f t="shared" si="2"/>
@@ -5523,7 +5514,7 @@
         <v>95</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
@@ -5547,7 +5538,7 @@
         <v>96</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
@@ -5571,7 +5562,7 @@
         <v>97</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
@@ -5595,7 +5586,7 @@
         <v>98</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
@@ -5619,7 +5610,7 @@
         <v>99</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
@@ -5643,7 +5634,7 @@
         <v>100</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
@@ -5667,7 +5658,7 @@
         <v>101</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -5691,7 +5682,7 @@
         <v>102</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -5715,7 +5706,7 @@
         <v>103</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -5739,7 +5730,7 @@
         <v>104</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -5763,7 +5754,7 @@
         <v>105</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -5787,7 +5778,7 @@
         <v>106</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -5811,7 +5802,7 @@
         <v>107</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -5835,7 +5826,7 @@
         <v>108</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -5859,7 +5850,7 @@
         <v>109</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -5883,7 +5874,7 @@
         <v>110</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -5907,7 +5898,7 @@
         <v>111</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -5931,7 +5922,7 @@
         <v>112</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -5955,7 +5946,7 @@
         <v>113</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -5979,7 +5970,7 @@
         <v>114</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -6003,7 +5994,7 @@
         <v>115</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -6027,7 +6018,7 @@
         <v>116</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -6051,7 +6042,7 @@
         <v>117</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -6075,11 +6066,19 @@
         <v>118</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="X2:AA3"/>
+    <mergeCell ref="X6:AA7"/>
+    <mergeCell ref="W1:AB1"/>
+    <mergeCell ref="X4:AA5"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:N1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="S1:V1"/>
     <mergeCell ref="X20:AA21"/>
     <mergeCell ref="X22:AA23"/>
     <mergeCell ref="X24:AA25"/>
@@ -6089,14 +6088,6 @@
     <mergeCell ref="X13:AA14"/>
     <mergeCell ref="X15:AA16"/>
     <mergeCell ref="X17:AA18"/>
-    <mergeCell ref="X2:AA3"/>
-    <mergeCell ref="X6:AA7"/>
-    <mergeCell ref="W1:AB1"/>
-    <mergeCell ref="X4:AA5"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:N1"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="S1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6120,33 +6111,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16" t="s">
+      <c r="A1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16" t="s">
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61" t="s">
         <v>120</v>
       </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">

</xml_diff>